<commit_message>
modified:   Band2MaxPowerInput1_FrequencySweepRanges.xlsx 	modified:   FSW_test_5ranges.py
</commit_message>
<xml_diff>
--- a/Band2MaxPowerInput1_FrequencySweepRanges.xlsx
+++ b/Band2MaxPowerInput1_FrequencySweepRanges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\DVT-Wireless-HCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A424CF-ED59-49B8-AFD1-495F34625675}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130D205E-C72F-4CBD-8C1F-84FA3720CD0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
   </bookViews>
   <sheets>
     <sheet name="Band2" sheetId="1" r:id="rId1"/>
@@ -542,7 +542,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -634,6 +634,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -956,7 +962,7 @@
   <dimension ref="A1:AL28"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1048576"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3767,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855F8828-1D8C-4AAA-81FD-7AC3397EB1C9}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1048576"/>
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5580,7 +5586,7 @@
   <dimension ref="A1:V60"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1048576"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7418,7 +7424,7 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1048576"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9230,8 +9236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDABD784-AD31-46F2-99DC-A4DD1B41AE1B}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1048576"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10096,8 +10102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7206B6-36E5-4637-B4E1-0FEA65E91330}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1048576"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10111,7 +10117,7 @@
     <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.85546875" style="79" customWidth="1"/>
+    <col min="19" max="20" width="12.85546875" style="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -10169,10 +10175,10 @@
       <c r="R1" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="77" t="s">
+      <c r="S1" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="T1" s="77" t="s">
+      <c r="T1" s="81" t="s">
         <v>93</v>
       </c>
       <c r="U1" s="67" t="s">
@@ -10240,10 +10246,10 @@
         <f>C2-400</f>
         <v>1710.6999999999998</v>
       </c>
-      <c r="S2" s="78">
+      <c r="S2" s="82">
         <v>4.47</v>
       </c>
-      <c r="T2" s="78">
+      <c r="T2" s="82">
         <v>5.61</v>
       </c>
       <c r="U2">
@@ -10310,10 +10316,10 @@
         <f t="shared" ref="R3:R28" si="0">C3-400</f>
         <v>1710.6999999999998</v>
       </c>
-      <c r="S3" s="78">
+      <c r="S3" s="82">
         <v>4.47</v>
       </c>
-      <c r="T3" s="78">
+      <c r="T3" s="82">
         <v>5.61</v>
       </c>
     </row>
@@ -10373,10 +10379,10 @@
         <f t="shared" si="0"/>
         <v>1710.6999999999998</v>
       </c>
-      <c r="S4" s="78">
+      <c r="S4" s="82">
         <v>4.47</v>
       </c>
-      <c r="T4" s="78">
+      <c r="T4" s="82">
         <v>5.61</v>
       </c>
     </row>
@@ -10436,10 +10442,10 @@
         <f t="shared" si="0"/>
         <v>1712.5</v>
       </c>
-      <c r="S5" s="78">
+      <c r="S5" s="82">
         <v>4.4800000000000004</v>
       </c>
-      <c r="T5" s="78">
+      <c r="T5" s="82">
         <v>5.62</v>
       </c>
     </row>
@@ -10499,10 +10505,10 @@
         <f t="shared" si="0"/>
         <v>1712.5</v>
       </c>
-      <c r="S6" s="78">
+      <c r="S6" s="82">
         <v>4.4800000000000004</v>
       </c>
-      <c r="T6" s="78">
+      <c r="T6" s="82">
         <v>5.62</v>
       </c>
     </row>
@@ -10562,10 +10568,10 @@
         <f t="shared" si="0"/>
         <v>1712.5</v>
       </c>
-      <c r="S7" s="78">
+      <c r="S7" s="82">
         <v>4.4800000000000004</v>
       </c>
-      <c r="T7" s="78">
+      <c r="T7" s="82">
         <v>5.62</v>
       </c>
     </row>
@@ -10625,10 +10631,10 @@
         <f t="shared" si="0"/>
         <v>1720</v>
       </c>
-      <c r="S8" s="78">
+      <c r="S8" s="82">
         <v>4.5</v>
       </c>
-      <c r="T8" s="78">
+      <c r="T8" s="82">
         <v>5.64</v>
       </c>
     </row>
@@ -10688,10 +10694,10 @@
         <f t="shared" si="0"/>
         <v>1720</v>
       </c>
-      <c r="S9" s="78">
+      <c r="S9" s="82">
         <v>4.5</v>
       </c>
-      <c r="T9" s="78">
+      <c r="T9" s="82">
         <v>5.64</v>
       </c>
     </row>
@@ -10751,10 +10757,10 @@
         <f t="shared" si="0"/>
         <v>1720</v>
       </c>
-      <c r="S10" s="78">
+      <c r="S10" s="82">
         <v>4.5</v>
       </c>
-      <c r="T10" s="78">
+      <c r="T10" s="82">
         <v>5.64</v>
       </c>
     </row>
@@ -10814,10 +10820,10 @@
         <f t="shared" si="0"/>
         <v>1745</v>
       </c>
-      <c r="S11" s="78">
+      <c r="S11" s="82">
         <v>4.57</v>
       </c>
-      <c r="T11" s="78">
+      <c r="T11" s="82">
         <v>5.71</v>
       </c>
     </row>
@@ -10877,10 +10883,10 @@
         <f t="shared" si="0"/>
         <v>1745</v>
       </c>
-      <c r="S12" s="78">
+      <c r="S12" s="82">
         <v>4.57</v>
       </c>
-      <c r="T12" s="78">
+      <c r="T12" s="82">
         <v>5.71</v>
       </c>
     </row>
@@ -10940,10 +10946,10 @@
         <f t="shared" si="0"/>
         <v>1745</v>
       </c>
-      <c r="S13" s="78">
+      <c r="S13" s="82">
         <v>4.57</v>
       </c>
-      <c r="T13" s="78">
+      <c r="T13" s="82">
         <v>5.71</v>
       </c>
     </row>
@@ -11003,10 +11009,10 @@
         <f t="shared" si="0"/>
         <v>1745</v>
       </c>
-      <c r="S14" s="78">
+      <c r="S14" s="82">
         <v>4.57</v>
       </c>
-      <c r="T14" s="78">
+      <c r="T14" s="82">
         <v>5.71</v>
       </c>
     </row>
@@ -11066,10 +11072,10 @@
         <f t="shared" si="0"/>
         <v>1745</v>
       </c>
-      <c r="S15" s="78">
+      <c r="S15" s="82">
         <v>4.57</v>
       </c>
-      <c r="T15" s="78">
+      <c r="T15" s="82">
         <v>5.71</v>
       </c>
     </row>
@@ -11129,10 +11135,10 @@
         <f t="shared" si="0"/>
         <v>1745</v>
       </c>
-      <c r="S16" s="78">
+      <c r="S16" s="82">
         <v>4.57</v>
       </c>
-      <c r="T16" s="78">
+      <c r="T16" s="82">
         <v>5.71</v>
       </c>
     </row>
@@ -11192,10 +11198,10 @@
         <f t="shared" si="0"/>
         <v>1745</v>
       </c>
-      <c r="S17" s="78">
+      <c r="S17" s="82">
         <v>4.57</v>
       </c>
-      <c r="T17" s="78">
+      <c r="T17" s="82">
         <v>5.71</v>
       </c>
     </row>
@@ -11255,10 +11261,10 @@
         <f t="shared" si="0"/>
         <v>1745</v>
       </c>
-      <c r="S18" s="78">
+      <c r="S18" s="82">
         <v>4.57</v>
       </c>
-      <c r="T18" s="78">
+      <c r="T18" s="82">
         <v>5.71</v>
       </c>
     </row>
@@ -11318,10 +11324,10 @@
         <f t="shared" si="0"/>
         <v>1745</v>
       </c>
-      <c r="S19" s="78">
+      <c r="S19" s="82">
         <v>4.57</v>
       </c>
-      <c r="T19" s="78">
+      <c r="T19" s="82">
         <v>5.71</v>
       </c>
     </row>
@@ -11381,10 +11387,10 @@
         <f t="shared" si="0"/>
         <v>1779.3000000000002</v>
       </c>
-      <c r="S20" s="78">
+      <c r="S20" s="82">
         <v>4.67</v>
       </c>
-      <c r="T20" s="78">
+      <c r="T20" s="82">
         <v>5.81</v>
       </c>
     </row>
@@ -11444,10 +11450,10 @@
         <f t="shared" si="0"/>
         <v>1779.3000000000002</v>
       </c>
-      <c r="S21" s="78">
+      <c r="S21" s="82">
         <v>4.67</v>
       </c>
-      <c r="T21" s="78">
+      <c r="T21" s="82">
         <v>5.81</v>
       </c>
     </row>
@@ -11507,10 +11513,10 @@
         <f t="shared" si="0"/>
         <v>1779.3000000000002</v>
       </c>
-      <c r="S22" s="78">
+      <c r="S22" s="82">
         <v>4.67</v>
       </c>
-      <c r="T22" s="78">
+      <c r="T22" s="82">
         <v>5.81</v>
       </c>
     </row>
@@ -11570,10 +11576,10 @@
         <f t="shared" si="0"/>
         <v>1777.5</v>
       </c>
-      <c r="S23" s="78">
+      <c r="S23" s="82">
         <v>4.66</v>
       </c>
-      <c r="T23" s="78">
+      <c r="T23" s="82">
         <v>5.8</v>
       </c>
     </row>
@@ -11633,10 +11639,10 @@
         <f t="shared" si="0"/>
         <v>1777.5</v>
       </c>
-      <c r="S24" s="78">
+      <c r="S24" s="82">
         <v>4.66</v>
       </c>
-      <c r="T24" s="78">
+      <c r="T24" s="82">
         <v>5.8</v>
       </c>
     </row>
@@ -11696,10 +11702,10 @@
         <f t="shared" si="0"/>
         <v>1777.5</v>
       </c>
-      <c r="S25" s="78">
+      <c r="S25" s="82">
         <v>4.66</v>
       </c>
-      <c r="T25" s="78">
+      <c r="T25" s="82">
         <v>5.8</v>
       </c>
     </row>
@@ -11759,10 +11765,10 @@
         <f t="shared" si="0"/>
         <v>1770</v>
       </c>
-      <c r="S26" s="78">
+      <c r="S26" s="82">
         <v>4.6399999999999997</v>
       </c>
-      <c r="T26" s="78">
+      <c r="T26" s="82">
         <v>5.78</v>
       </c>
     </row>
@@ -11822,10 +11828,10 @@
         <f t="shared" si="0"/>
         <v>1770</v>
       </c>
-      <c r="S27" s="78">
+      <c r="S27" s="82">
         <v>4.6399999999999997</v>
       </c>
-      <c r="T27" s="78">
+      <c r="T27" s="82">
         <v>5.78</v>
       </c>
     </row>
@@ -11885,10 +11891,10 @@
         <f t="shared" si="0"/>
         <v>1770</v>
       </c>
-      <c r="S28" s="78">
+      <c r="S28" s="82">
         <v>4.6399999999999997</v>
       </c>
-      <c r="T28" s="78">
+      <c r="T28" s="82">
         <v>5.78</v>
       </c>
     </row>

</xml_diff>